<commit_message>
generación informe prueba json
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>fecha</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>correo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +469,11 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>20 febrero 2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>carlos.velez@est.iudigital.edu.co</t>
         </is>
       </c>
     </row>

</xml_diff>